<commit_message>
Halved the Shwedagon Paya's cost and restricted it to coastal cities with a nearby Rainforest or Jungle
Moved Vietnamese Core 2W

Added Burma - 650 AD in Pagan. Core includes Pagan and Bassien
Huge credit goes to Merijn and History Rewritten for the base concept and implementation, respectively

UP - The Power of Monks Kings: Religious buildings provide +1 Great Person Point
UU - Kyundaw: Replaces Heavy Spearmen, can move through Rainforests, Jungles, and Marshes, starts with City Raider I, +25% Rainforest Attack
UB - Paya: Replaces Library, +1 Artist Slot, +1 Priest Slot

UHV1 - Indochinese Buddhism: Build the Shwedagon Paya, 2 Buddhist Temples, and 2 Buddhist Monasteries by 1000 AD
UHV2 - The Five Temples: Have at least one Great Priest, Great Scientist and Great Artist settled in your cities in 1211 AD
UHV3 - The Toungoo Dynasty: Control all of Indochina in 1580 AD
</commit_message>
<xml_diff>
--- a/Assets/Python/Modifiers.xlsx
+++ b/Assets/Python/Modifiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Civ4\Beyond the Sword\Mods\RFC Dawn of Civilization\Assets\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86B322A4-2734-4C71-8F9F-4B1ACC095F5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CCC725-888E-45FA-8CC8-50DB22D17C52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7801921E-5EA5-45CA-A791-B19681F4808F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -192,9 +192,6 @@
     <t>BAR</t>
   </si>
   <si>
-    <t xml:space="preserve"> )</t>
-  </si>
-  <si>
     <t xml:space="preserve">tCulture = ( </t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>BOE</t>
+  </si>
+  <si>
+    <t>BUR</t>
   </si>
 </sst>
 </file>
@@ -615,13 +615,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B40B88-620F-4807-8C81-450C4EB3ED4C}">
   <dimension ref="A1:BN22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:BN17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
@@ -668,7 +669,7 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
@@ -695,135 +696,138 @@
         <v>21</v>
       </c>
       <c r="X1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG1" t="s">
         <v>68</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>69</v>
       </c>
-      <c r="AG1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO1" t="s">
         <v>71</v>
       </c>
-      <c r="AK1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AW1" t="s">
         <v>72</v>
       </c>
-      <c r="AO1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY1" t="s">
         <v>73</v>
       </c>
-      <c r="AW1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF1" t="s">
         <v>74</v>
       </c>
-      <c r="AY1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>76</v>
-      </c>
       <c r="BG1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH1" t="s">
         <v>48</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>6</v>
       </c>
       <c r="BI1" t="s">
         <v>6</v>
       </c>
       <c r="BJ1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BK1" t="s">
         <v>49</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>50</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>51</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>90</v>
@@ -892,97 +896,97 @@
         <v>120</v>
       </c>
       <c r="X3">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="Y3">
         <v>125</v>
       </c>
       <c r="Z3">
+        <v>125</v>
+      </c>
+      <c r="AA3">
         <v>160</v>
       </c>
-      <c r="AA3">
-        <v>120</v>
-      </c>
       <c r="AB3">
+        <v>120</v>
+      </c>
+      <c r="AC3">
         <v>130</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>150</v>
-      </c>
-      <c r="AD3">
-        <v>130</v>
       </c>
       <c r="AE3">
         <v>130</v>
       </c>
       <c r="AF3">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="AG3">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="AH3">
         <v>130</v>
       </c>
       <c r="AI3">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="AJ3">
+        <v>110</v>
+      </c>
+      <c r="AK3">
         <v>130</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>147</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>140</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>150</v>
       </c>
-      <c r="AN3">
-        <v>120</v>
-      </c>
       <c r="AO3">
+        <v>120</v>
+      </c>
+      <c r="AP3">
         <v>135</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>140</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>125</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>150</v>
-      </c>
-      <c r="AS3">
-        <v>130</v>
       </c>
       <c r="AT3">
         <v>130</v>
       </c>
       <c r="AU3">
+        <v>130</v>
+      </c>
+      <c r="AV3">
         <v>135</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>140</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>165</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>140</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>150</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>140</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>130</v>
-      </c>
-      <c r="BB3">
-        <v>140</v>
       </c>
       <c r="BC3">
         <v>140</v>
@@ -1000,7 +1004,7 @@
         <v>140</v>
       </c>
       <c r="BH3">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="BI3">
         <v>20</v>
@@ -1009,21 +1013,21 @@
         <v>20</v>
       </c>
       <c r="BK3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="BL3">
         <v>50</v>
       </c>
       <c r="BM3">
+        <v>50</v>
+      </c>
+      <c r="BN3">
         <v>30</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>135</v>
@@ -1092,19 +1096,19 @@
         <v>100</v>
       </c>
       <c r="X5">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="Y5">
         <v>110</v>
       </c>
       <c r="Z5">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AA5">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AB5">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AC5">
         <v>100</v>
@@ -1140,31 +1144,31 @@
         <v>100</v>
       </c>
       <c r="AN5">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AO5">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="AP5">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="AQ5">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="AR5">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AS5">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="AT5">
         <v>90</v>
       </c>
       <c r="AU5">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="AV5">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="AW5">
         <v>90</v>
@@ -1173,22 +1177,22 @@
         <v>90</v>
       </c>
       <c r="AY5">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="AZ5">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="BA5">
         <v>80</v>
       </c>
       <c r="BB5">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="BC5">
         <v>90</v>
       </c>
       <c r="BD5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="BE5">
         <v>80</v>
@@ -1197,33 +1201,33 @@
         <v>80</v>
       </c>
       <c r="BG5">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="BH5">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="BI5">
         <v>0</v>
       </c>
       <c r="BJ5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="BK5">
         <v>100</v>
       </c>
       <c r="BL5">
+        <v>100</v>
+      </c>
+      <c r="BM5">
         <v>50</v>
       </c>
-      <c r="BM5">
-        <v>100</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>53</v>
+      <c r="BN5">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>140</v>
@@ -1292,97 +1296,97 @@
         <v>100</v>
       </c>
       <c r="X6">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="Y6">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="Z6">
         <v>80</v>
       </c>
       <c r="AA6">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AB6">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AC6">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AD6">
+        <v>100</v>
+      </c>
+      <c r="AE6">
         <v>85</v>
       </c>
-      <c r="AE6">
-        <v>100</v>
-      </c>
       <c r="AF6">
         <v>100</v>
       </c>
       <c r="AG6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AH6">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="AI6">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="AJ6">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AK6">
+        <v>100</v>
+      </c>
+      <c r="AL6">
         <v>85</v>
       </c>
-      <c r="AL6">
-        <v>80</v>
-      </c>
       <c r="AM6">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AN6">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="AO6">
         <v>90</v>
       </c>
       <c r="AP6">
+        <v>90</v>
+      </c>
+      <c r="AQ6">
         <v>85</v>
       </c>
-      <c r="AQ6">
-        <v>120</v>
-      </c>
       <c r="AR6">
         <v>120</v>
       </c>
       <c r="AS6">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="AT6">
+        <v>100</v>
+      </c>
+      <c r="AU6">
         <v>85</v>
       </c>
-      <c r="AU6">
-        <v>110</v>
-      </c>
       <c r="AV6">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="AW6">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AX6">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AY6">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="AZ6">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="BA6">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="BB6">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="BC6">
         <v>90</v>
@@ -1391,16 +1395,16 @@
         <v>90</v>
       </c>
       <c r="BE6">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="BF6">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="BG6">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="BH6">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="BI6">
         <v>110</v>
@@ -1409,21 +1413,21 @@
         <v>110</v>
       </c>
       <c r="BK6">
+        <v>110</v>
+      </c>
+      <c r="BL6">
         <v>350</v>
       </c>
-      <c r="BL6">
-        <v>110</v>
-      </c>
       <c r="BM6">
         <v>110</v>
       </c>
-      <c r="BN6" t="s">
-        <v>53</v>
+      <c r="BN6">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -1495,29 +1499,29 @@
         <v>80</v>
       </c>
       <c r="Y7">
+        <v>80</v>
+      </c>
+      <c r="Z7">
         <v>55</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>65</v>
       </c>
-      <c r="AA7">
-        <v>80</v>
-      </c>
       <c r="AB7">
+        <v>80</v>
+      </c>
+      <c r="AC7">
         <v>55</v>
       </c>
-      <c r="AC7">
-        <v>70</v>
-      </c>
       <c r="AD7">
         <v>70</v>
       </c>
       <c r="AE7">
+        <v>70</v>
+      </c>
+      <c r="AF7">
         <v>65</v>
       </c>
-      <c r="AF7">
-        <v>80</v>
-      </c>
       <c r="AG7">
         <v>80</v>
       </c>
@@ -1525,46 +1529,46 @@
         <v>80</v>
       </c>
       <c r="AI7">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AJ7">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AK7">
         <v>80</v>
       </c>
       <c r="AL7">
+        <v>80</v>
+      </c>
+      <c r="AM7">
         <v>60</v>
       </c>
-      <c r="AM7">
-        <v>70</v>
-      </c>
       <c r="AN7">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AO7">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AP7">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AQ7">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="AR7">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="AS7">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="AT7">
         <v>80</v>
       </c>
       <c r="AU7">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AV7">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="AW7">
         <v>70</v>
@@ -1573,34 +1577,34 @@
         <v>70</v>
       </c>
       <c r="AY7">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AZ7">
+        <v>80</v>
+      </c>
+      <c r="BA7">
         <v>60</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>50</v>
       </c>
-      <c r="BB7">
-        <v>70</v>
-      </c>
       <c r="BC7">
         <v>70</v>
       </c>
       <c r="BD7">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="BE7">
+        <v>80</v>
+      </c>
+      <c r="BF7">
         <v>60</v>
       </c>
-      <c r="BF7">
-        <v>80</v>
-      </c>
       <c r="BG7">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="BH7">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="BI7">
         <v>20</v>
@@ -1617,13 +1621,13 @@
       <c r="BM7">
         <v>20</v>
       </c>
-      <c r="BN7" t="s">
-        <v>53</v>
+      <c r="BN7">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>135</v>
@@ -1692,28 +1696,28 @@
         <v>100</v>
       </c>
       <c r="X8">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="Y8">
+        <v>70</v>
+      </c>
+      <c r="Z8">
         <v>50</v>
       </c>
-      <c r="Z8">
-        <v>70</v>
-      </c>
       <c r="AA8">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="AB8">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="AC8">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AD8">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AE8">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="AF8">
         <v>90</v>
@@ -1725,82 +1729,82 @@
         <v>90</v>
       </c>
       <c r="AI8">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="AJ8">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="AK8">
         <v>85</v>
       </c>
       <c r="AL8">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AM8">
         <v>80</v>
       </c>
       <c r="AN8">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AO8">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="AP8">
+        <v>75</v>
+      </c>
+      <c r="AQ8">
         <v>85</v>
       </c>
-      <c r="AQ8">
-        <v>100</v>
-      </c>
       <c r="AR8">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="AS8">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="AT8">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AU8">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AV8">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="AW8">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AX8">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AY8">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AZ8">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="BA8">
+        <v>70</v>
+      </c>
+      <c r="BB8">
         <v>50</v>
-      </c>
-      <c r="BB8">
-        <v>85</v>
       </c>
       <c r="BC8">
         <v>85</v>
       </c>
       <c r="BD8">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="BE8">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="BF8">
         <v>70</v>
       </c>
       <c r="BG8">
+        <v>70</v>
+      </c>
+      <c r="BH8">
         <v>60</v>
-      </c>
-      <c r="BH8">
-        <v>30</v>
       </c>
       <c r="BI8">
         <v>30</v>
@@ -1817,13 +1821,13 @@
       <c r="BM8">
         <v>30</v>
       </c>
-      <c r="BN8" t="s">
-        <v>53</v>
+      <c r="BN8">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>120</v>
@@ -1892,25 +1896,25 @@
         <v>100</v>
       </c>
       <c r="X9">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="Y9">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="Z9">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AA9">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AB9">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="AC9">
         <v>70</v>
       </c>
       <c r="AD9">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AE9">
         <v>80</v>
@@ -1925,37 +1929,37 @@
         <v>80</v>
       </c>
       <c r="AI9">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AJ9">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AK9">
         <v>80</v>
       </c>
       <c r="AL9">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="AM9">
         <v>60</v>
       </c>
       <c r="AN9">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AO9">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AP9">
         <v>60</v>
       </c>
       <c r="AQ9">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="AR9">
         <v>90</v>
       </c>
       <c r="AS9">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AT9">
         <v>80</v>
@@ -1964,7 +1968,7 @@
         <v>80</v>
       </c>
       <c r="AV9">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AW9">
         <v>70</v>
@@ -1973,34 +1977,34 @@
         <v>70</v>
       </c>
       <c r="AY9">
+        <v>70</v>
+      </c>
+      <c r="AZ9">
         <v>60</v>
-      </c>
-      <c r="AZ9">
-        <v>50</v>
       </c>
       <c r="BA9">
         <v>50</v>
       </c>
       <c r="BB9">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="BC9">
         <v>70</v>
       </c>
       <c r="BD9">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="BE9">
         <v>75</v>
       </c>
       <c r="BF9">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="BG9">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="BH9">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="BI9">
         <v>70</v>
@@ -2017,13 +2021,13 @@
       <c r="BM9">
         <v>70</v>
       </c>
-      <c r="BN9" t="s">
-        <v>53</v>
+      <c r="BN9">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -2092,7 +2096,7 @@
         <v>3</v>
       </c>
       <c r="X10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y10">
         <v>2</v>
@@ -2101,10 +2105,10 @@
         <v>2</v>
       </c>
       <c r="AA10">
+        <v>2</v>
+      </c>
+      <c r="AB10">
         <v>3</v>
-      </c>
-      <c r="AB10">
-        <v>2</v>
       </c>
       <c r="AC10">
         <v>2</v>
@@ -2128,28 +2132,28 @@
         <v>2</v>
       </c>
       <c r="AJ10">
+        <v>2</v>
+      </c>
+      <c r="AK10">
         <v>3</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>2</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <v>3</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>2</v>
       </c>
-      <c r="AN10">
+      <c r="AO10">
         <v>4</v>
-      </c>
-      <c r="AO10">
-        <v>3</v>
       </c>
       <c r="AP10">
         <v>3</v>
       </c>
       <c r="AQ10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AR10">
         <v>4</v>
@@ -2161,7 +2165,7 @@
         <v>4</v>
       </c>
       <c r="AU10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AV10">
         <v>3</v>
@@ -2200,7 +2204,7 @@
         <v>3</v>
       </c>
       <c r="BH10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BI10">
         <v>0</v>
@@ -2217,13 +2221,13 @@
       <c r="BM10">
         <v>0</v>
       </c>
-      <c r="BN10" t="s">
-        <v>53</v>
+      <c r="BN10">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>110</v>
@@ -2292,10 +2296,10 @@
         <v>105</v>
       </c>
       <c r="X12">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Y12">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="Z12">
         <v>90</v>
@@ -2304,10 +2308,10 @@
         <v>90</v>
       </c>
       <c r="AB12">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AC12">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AD12">
         <v>90</v>
@@ -2325,28 +2329,28 @@
         <v>90</v>
       </c>
       <c r="AI12">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AJ12">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AK12">
         <v>90</v>
       </c>
       <c r="AL12">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AM12">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="AN12">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="AO12">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AP12">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AQ12">
         <v>100</v>
@@ -2355,13 +2359,13 @@
         <v>100</v>
       </c>
       <c r="AS12">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AT12">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="AU12">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="AV12">
         <v>90</v>
@@ -2373,16 +2377,16 @@
         <v>90</v>
       </c>
       <c r="AY12">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="AZ12">
+        <v>75</v>
+      </c>
+      <c r="BA12">
         <v>85</v>
       </c>
-      <c r="BA12">
-        <v>80</v>
-      </c>
       <c r="BB12">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="BC12">
         <v>85</v>
@@ -2400,30 +2404,30 @@
         <v>85</v>
       </c>
       <c r="BH12">
-        <v>200</v>
+        <v>85</v>
       </c>
       <c r="BI12">
         <v>200</v>
       </c>
       <c r="BJ12">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="BK12">
         <v>150</v>
       </c>
       <c r="BL12">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="BM12">
+        <v>100</v>
+      </c>
+      <c r="BN12">
         <v>140</v>
-      </c>
-      <c r="BN12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13">
         <v>80</v>
@@ -2492,97 +2496,97 @@
         <v>80</v>
       </c>
       <c r="X13">
+        <v>90</v>
+      </c>
+      <c r="Y13">
         <v>85</v>
       </c>
-      <c r="Y13">
-        <v>90</v>
-      </c>
       <c r="Z13">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="AA13">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="AB13">
         <v>90</v>
       </c>
       <c r="AC13">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AD13">
         <v>100</v>
       </c>
       <c r="AE13">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AF13">
         <v>90</v>
       </c>
       <c r="AG13">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="AH13">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="AI13">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AJ13">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AK13">
         <v>90</v>
       </c>
       <c r="AL13">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AM13">
         <v>80</v>
       </c>
       <c r="AN13">
+        <v>80</v>
+      </c>
+      <c r="AO13">
         <v>85</v>
       </c>
-      <c r="AO13">
-        <v>90</v>
-      </c>
       <c r="AP13">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AQ13">
         <v>80</v>
       </c>
       <c r="AR13">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AS13">
         <v>90</v>
       </c>
       <c r="AT13">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AU13">
+        <v>100</v>
+      </c>
+      <c r="AV13">
         <v>85</v>
       </c>
-      <c r="AV13">
-        <v>90</v>
-      </c>
       <c r="AW13">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="AX13">
         <v>100</v>
       </c>
       <c r="AY13">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AZ13">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="BA13">
         <v>70</v>
       </c>
       <c r="BB13">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="BC13">
         <v>90</v>
@@ -2591,16 +2595,16 @@
         <v>90</v>
       </c>
       <c r="BE13">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="BF13">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="BG13">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="BH13">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="BI13">
         <v>150</v>
@@ -2609,7 +2613,7 @@
         <v>150</v>
       </c>
       <c r="BK13">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="BL13">
         <v>100</v>
@@ -2617,13 +2621,13 @@
       <c r="BM13">
         <v>100</v>
       </c>
-      <c r="BN13" t="s">
-        <v>53</v>
+      <c r="BN13">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>110</v>
@@ -2698,46 +2702,46 @@
         <v>90</v>
       </c>
       <c r="Z14">
+        <v>90</v>
+      </c>
+      <c r="AA14">
         <v>85</v>
       </c>
-      <c r="AA14">
-        <v>100</v>
-      </c>
       <c r="AB14">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AC14">
+        <v>90</v>
+      </c>
+      <c r="AD14">
         <v>85</v>
       </c>
-      <c r="AD14">
-        <v>90</v>
-      </c>
       <c r="AE14">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AF14">
         <v>80</v>
       </c>
       <c r="AG14">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AH14">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI14">
         <v>80</v>
       </c>
       <c r="AJ14">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AK14">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AL14">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AM14">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AN14">
         <v>80</v>
@@ -2749,11 +2753,11 @@
         <v>80</v>
       </c>
       <c r="AQ14">
+        <v>80</v>
+      </c>
+      <c r="AR14">
         <v>85</v>
       </c>
-      <c r="AR14">
-        <v>80</v>
-      </c>
       <c r="AS14">
         <v>80</v>
       </c>
@@ -2770,10 +2774,10 @@
         <v>80</v>
       </c>
       <c r="AX14">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AY14">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AZ14">
         <v>70</v>
@@ -2782,48 +2786,48 @@
         <v>70</v>
       </c>
       <c r="BB14">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="BC14">
         <v>80</v>
       </c>
       <c r="BD14">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="BE14">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="BF14">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="BG14">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="BH14">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="BI14">
         <v>100</v>
       </c>
       <c r="BJ14">
+        <v>100</v>
+      </c>
+      <c r="BK14">
         <v>150</v>
       </c>
-      <c r="BK14">
-        <v>100</v>
-      </c>
       <c r="BL14">
         <v>100</v>
       </c>
       <c r="BM14">
         <v>100</v>
       </c>
-      <c r="BN14" t="s">
-        <v>53</v>
+      <c r="BN14">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15">
         <v>130</v>
@@ -2892,103 +2896,103 @@
         <v>90</v>
       </c>
       <c r="X15">
+        <v>100</v>
+      </c>
+      <c r="Y15">
         <v>85</v>
       </c>
-      <c r="Y15">
-        <v>90</v>
-      </c>
       <c r="Z15">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="AA15">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="AB15">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="AC15">
         <v>70</v>
       </c>
       <c r="AD15">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AE15">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="AF15">
+        <v>100</v>
+      </c>
+      <c r="AG15">
         <v>115</v>
       </c>
-      <c r="AG15">
-        <v>75</v>
-      </c>
       <c r="AH15">
+        <v>75</v>
+      </c>
+      <c r="AI15">
         <v>115</v>
       </c>
-      <c r="AI15">
-        <v>70</v>
-      </c>
       <c r="AJ15">
+        <v>70</v>
+      </c>
+      <c r="AK15">
         <v>85</v>
       </c>
-      <c r="AK15">
-        <v>80</v>
-      </c>
       <c r="AL15">
         <v>80</v>
       </c>
       <c r="AM15">
+        <v>80</v>
+      </c>
+      <c r="AN15">
         <v>85</v>
       </c>
-      <c r="AN15">
-        <v>75</v>
-      </c>
       <c r="AO15">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="AP15">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AQ15">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AR15">
         <v>100</v>
       </c>
       <c r="AS15">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="AT15">
         <v>75</v>
       </c>
       <c r="AU15">
+        <v>75</v>
+      </c>
+      <c r="AV15">
         <v>85</v>
       </c>
-      <c r="AV15">
-        <v>75</v>
-      </c>
       <c r="AW15">
+        <v>75</v>
+      </c>
+      <c r="AX15">
         <v>85</v>
       </c>
-      <c r="AX15">
-        <v>90</v>
-      </c>
       <c r="AY15">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="AZ15">
+        <v>70</v>
+      </c>
+      <c r="BA15">
         <v>65</v>
       </c>
-      <c r="BA15">
+      <c r="BB15">
         <v>60</v>
-      </c>
-      <c r="BB15">
-        <v>65</v>
       </c>
       <c r="BC15">
         <v>65</v>
       </c>
       <c r="BD15">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="BE15">
         <v>60</v>
@@ -3000,7 +3004,7 @@
         <v>60</v>
       </c>
       <c r="BH15">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="BI15">
         <v>95</v>
@@ -3017,13 +3021,13 @@
       <c r="BM15">
         <v>95</v>
       </c>
-      <c r="BN15" t="s">
-        <v>53</v>
+      <c r="BN15">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:66" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16">
         <v>140</v>
@@ -3092,22 +3096,22 @@
         <v>90</v>
       </c>
       <c r="X16">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="Y16">
         <v>75</v>
       </c>
       <c r="Z16">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AA16">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="AB16">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="AC16">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AD16">
         <v>80</v>
@@ -3131,40 +3135,40 @@
         <v>80</v>
       </c>
       <c r="AK16">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AL16">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AM16">
+        <v>70</v>
+      </c>
+      <c r="AN16">
         <v>65</v>
       </c>
-      <c r="AN16">
+      <c r="AO16">
         <v>85</v>
       </c>
-      <c r="AO16">
-        <v>70</v>
-      </c>
       <c r="AP16">
         <v>70</v>
       </c>
       <c r="AQ16">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AR16">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AS16">
         <v>80</v>
       </c>
       <c r="AT16">
+        <v>80</v>
+      </c>
+      <c r="AU16">
         <v>85</v>
       </c>
-      <c r="AU16">
-        <v>80</v>
-      </c>
       <c r="AV16">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AW16">
         <v>70</v>
@@ -3173,16 +3177,16 @@
         <v>70</v>
       </c>
       <c r="AY16">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="AZ16">
         <v>65</v>
       </c>
       <c r="BA16">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="BB16">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="BC16">
         <v>80</v>
@@ -3191,16 +3195,16 @@
         <v>80</v>
       </c>
       <c r="BE16">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="BF16">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="BG16">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="BH16">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="BI16">
         <v>100</v>
@@ -3217,13 +3221,13 @@
       <c r="BM16">
         <v>100</v>
       </c>
-      <c r="BN16" t="s">
-        <v>53</v>
+      <c r="BN16">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17">
         <v>150</v>
@@ -3304,10 +3308,10 @@
         <v>80</v>
       </c>
       <c r="AB17">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AC17">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AD17">
         <v>80</v>
@@ -3316,7 +3320,7 @@
         <v>80</v>
       </c>
       <c r="AF17">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AG17">
         <v>75</v>
@@ -3325,7 +3329,7 @@
         <v>75</v>
       </c>
       <c r="AI17">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AJ17">
         <v>80</v>
@@ -3334,19 +3338,19 @@
         <v>80</v>
       </c>
       <c r="AL17">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AM17">
         <v>70</v>
       </c>
       <c r="AN17">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AO17">
         <v>75</v>
       </c>
       <c r="AP17">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AQ17">
         <v>70</v>
@@ -3355,26 +3359,26 @@
         <v>70</v>
       </c>
       <c r="AS17">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AT17">
         <v>75</v>
       </c>
       <c r="AU17">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AV17">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AW17">
         <v>75</v>
       </c>
       <c r="AX17">
+        <v>75</v>
+      </c>
+      <c r="AY17">
         <v>65</v>
       </c>
-      <c r="AY17">
-        <v>70</v>
-      </c>
       <c r="AZ17">
         <v>70</v>
       </c>
@@ -3400,7 +3404,7 @@
         <v>70</v>
       </c>
       <c r="BH17">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="BI17">
         <v>125</v>
@@ -3417,8 +3421,8 @@
       <c r="BM17">
         <v>125</v>
       </c>
-      <c r="BN17" t="s">
-        <v>53</v>
+      <c r="BN17">
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>